<commit_message>
Allocate Wealth rebordering fail
From 2 to 3: G5:J7
</commit_message>
<xml_diff>
--- a/exe/2022_FinancialRecords - Kopie.xlsx
+++ b/exe/2022_FinancialRecords - Kopie.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="44">
   <si>
     <t>Income &amp; Expenses</t>
   </si>
@@ -137,6 +137,24 @@
   </si>
   <si>
     <t>Fixed</t>
+  </si>
+  <si>
+    <t>TER</t>
+  </si>
+  <si>
+    <t>NAHE</t>
+  </si>
+  <si>
+    <t>MUL</t>
+  </si>
+  <si>
+    <t>Fixed Asset</t>
+  </si>
+  <si>
+    <t>PERT</t>
+  </si>
+  <si>
+    <t>VLOR</t>
   </si>
 </sst>
 </file>
@@ -160,7 +178,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -227,19 +245,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -306,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -314,7 +319,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -324,15 +328,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="6" xfId="0" applyBorder="1"/>
-    <xf borderId="6" xfId="0" applyBorder="1"/>
-    <xf borderId="6" applyBorder="1"/>
+    <xf borderId="5" xfId="0" applyBorder="1"/>
+    <xf borderId="5" xfId="0" applyBorder="1"/>
+    <xf borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -610,7 +614,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A15" sqref="A15:N15"/>
@@ -622,22 +626,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.4">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="10"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="9"/>
     </row>
     <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
@@ -728,43 +732,43 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <f>SUM(Expenses!B:B)</f>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <f>SUM(Expenses!C:C)</f>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <f>SUM(Expenses!D:D)</f>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <f>SUM(Expenses!E:E)</f>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <f>SUM(Expenses!F:F)</f>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <f>SUM(Expenses!G:G)</f>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="4">
         <f>SUM(Expenses!H:H)</f>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="4">
         <f>SUM(Expenses!I:I)</f>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="4">
         <f>SUM(Expenses!J:J)</f>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="4">
         <f>SUM(Expenses!K:K)</f>
       </c>
-      <c r="L4" s="5">
+      <c r="L4" s="4">
         <f>SUM(Expenses!L:L)</f>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="4">
         <f>SUM(Expenses!M:M)</f>
       </c>
       <c r="N4" s="4">
@@ -772,77 +776,77 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15" x14ac:dyDescent="0.4">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
     </row>
     <row r="6" spans="1:14" ht="15" x14ac:dyDescent="0.4">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="10"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="9"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <f>B3+B4</f>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <f>C3+C4</f>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <f>D3+D4</f>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="6">
         <f>E3+E4</f>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="6">
         <f>F3+F4</f>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="6">
         <f>G3+G4</f>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="6">
         <f>H3+H4</f>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="6">
         <f>I3+I4</f>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="6">
         <f>J3+J4</f>
       </c>
-      <c r="K7" s="7">
+      <c r="K7" s="6">
         <f>K3+K4</f>
       </c>
-      <c r="L7" s="7">
+      <c r="L7" s="6">
         <f>L3+L4</f>
       </c>
-      <c r="M7" s="7">
+      <c r="M7" s="6">
         <f>M3+M4</f>
       </c>
       <c r="N7" s="4">
@@ -850,39 +854,39 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
     </row>
     <row r="9" spans="1:14" ht="15" x14ac:dyDescent="0.4"/>
     <row r="10" spans="1:14" ht="15" x14ac:dyDescent="0.4">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="10"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="9"/>
     </row>
     <row r="11" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
@@ -929,7 +933,9 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" s="4"/>
+      <c r="A12" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -945,7 +951,9 @@
       <c r="N12" s="4"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" s="4"/>
+      <c r="A13" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -961,157 +969,117 @@
       <c r="N13" s="4"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="A15" s="15"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="15"/>
-    </row>
-    <row r="16" spans="1:14">
-      <c r="A16" s="15"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-    </row>
-    <row r="17" spans="1:14">
-      <c r="A17" s="15"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
-    </row>
-    <row r="18" spans="1:14" ht="15" x14ac:dyDescent="0.4">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-    </row>
-    <row r="19" spans="1:14" ht="15" x14ac:dyDescent="0.4">
-      <c r="A19" s="8" t="s">
+      <c r="A14" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+    </row>
+    <row r="15" spans="1:14" ht="15" x14ac:dyDescent="0.4">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+    </row>
+    <row r="16" spans="1:14" ht="15" x14ac:dyDescent="0.4">
+      <c r="A16" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="10"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A22" s="5"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="9"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A17" s="6">
+        <f>A12</f>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A18" s="4">
+        <f>A13</f>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A19" s="4">
+        <f>A14</f>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="A6:N6"/>
     <mergeCell ref="A10:N10"/>
-    <mergeCell ref="A19:N19"/>
+    <mergeCell ref="A16:N16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.787402" bottom="0.787402" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1119,7 +1087,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
@@ -1132,25 +1100,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" x14ac:dyDescent="0.4">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="10"/>
-      <c r="G1" s="11" t="s">
+      <c r="D1" s="8"/>
+      <c r="E1" s="9"/>
+      <c r="G1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="9"/>
-      <c r="J1" s="10"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="9"/>
       <c r="L1" s="1" t="s">
         <v>22</v>
       </c>
@@ -1159,8 +1127,8 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" x14ac:dyDescent="0.4">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
       <c r="C2" s="1" t="s">
         <v>25</v>
       </c>
@@ -1170,7 +1138,7 @@
       <c r="E2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="12"/>
+      <c r="G2" s="11"/>
       <c r="H2" s="1" t="s">
         <v>25</v>
       </c>
@@ -1180,8 +1148,12 @@
       <c r="J2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
+      <c r="L2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" s="4">
+        <v>1010</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
@@ -1190,86 +1162,98 @@
       <c r="B3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>450</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>450</v>
       </c>
       <c r="E3" s="4">
         <f>D3-C3</f>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="4"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
+      <c r="G3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="4">
+        <v>455</v>
+      </c>
+      <c r="I3" s="4">
+        <v>455</v>
+      </c>
+      <c r="J3" s="4">
+        <f>I3-H3</f>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="M3" s="4">
+        <v>245</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>560</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>560</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <f>D4-C4</f>
       </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
+      <c r="G4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="4">
+        <v>555</v>
+      </c>
+      <c r="I4" s="4">
+        <v>555</v>
+      </c>
+      <c r="J4" s="4">
+        <f>I4-H4</f>
+      </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="12">
         <v>245</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="12">
         <v>245</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="12">
         <f>D5-C5</f>
       </c>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
+      <c r="G5" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="14">
+        <v>245</v>
+      </c>
+      <c r="I5" s="14">
+        <v>245</v>
+      </c>
+      <c r="J5" s="14">
+        <f>I5-H5</f>
+      </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1354,36 +1338,36 @@
       <c r="N2" s="4"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.787402" bottom="0.787402" header="0.3" footer="0.3"/>
@@ -1461,36 +1445,36 @@
       <c r="N2" s="4"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.787402" bottom="0.787402" header="0.3" footer="0.3"/>
@@ -1539,12 +1523,12 @@
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.787402" bottom="0.787402" header="0.3" footer="0.3"/>

</xml_diff>